<commit_message>
combined gui with class
</commit_message>
<xml_diff>
--- a/tkinter_excel_app/bid.xlsx
+++ b/tkinter_excel_app/bid.xlsx
@@ -15,7 +15,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -45,8 +47,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,10 +427,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -448,6 +451,122 @@
           <t>Seconds</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Bid end</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>204498232262</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>£</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>204498232262</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>£</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>204498232262</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>£</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>204498232262</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>£</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>45218.91527777778</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>175971859943</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>£</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>45218.91319444445</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>175971859943</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>£</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>45218.91527777778</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>